<commit_message>
update logic for new years
</commit_message>
<xml_diff>
--- a/Week1.xlsx
+++ b/Week1.xlsx
@@ -2373,7 +2373,11 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>4:45 AM MEET AT THE OFFICE</t>
+        </is>
+      </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr">
@@ -2430,7 +2434,11 @@
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>6:00 AM START</t>
+        </is>
+      </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2475,7 +2483,11 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2532,7 +2544,11 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>METCALFE'S MARKET #2600, WEST MADISON - LIFO</t>
+        </is>
+      </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
@@ -2589,7 +2605,11 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>7455 MINERAL POINT RD</t>
+        </is>
+      </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
@@ -2646,7 +2666,11 @@
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/NW4tsxQQBWF2</t>
+        </is>
+      </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
@@ -2767,9 +2791,21 @@
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>@ Store, Equip</t>
+        </is>
+      </c>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr">
@@ -2832,8 +2868,16 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Katherine</t>
+        </is>
+      </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
@@ -2885,9 +2929,22 @@
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Lashaun</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Driver,
+Prius</t>
+        </is>
+      </c>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr">
@@ -2938,9 +2995,21 @@
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Angela</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
@@ -2987,9 +3056,21 @@
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Anisha</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr">
         <is>
@@ -3040,9 +3121,21 @@
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Ashley P</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr">
         <is>
@@ -3083,9 +3176,21 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>7)</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>Eva</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr">
         <is>
@@ -3129,9 +3234,22 @@
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>8)</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Evelin</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>@ Store,
+After Liq Store</t>
+        </is>
+      </c>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr">
         <is>
@@ -3170,9 +3288,21 @@
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>9)</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr">
         <is>
@@ -3211,9 +3341,21 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>10)</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Lori</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr">
         <is>
@@ -3256,9 +3398,21 @@
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>11)</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Michael N</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr">
         <is>
@@ -3301,9 +3455,22 @@
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>12)</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Nate</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>@ Store,
+After Liq Store</t>
+        </is>
+      </c>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr">
         <is>
@@ -3342,9 +3509,21 @@
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>13)</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>Qiana</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr">
         <is>
@@ -3395,9 +3574,21 @@
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>14)</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>Savannah</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr">
         <is>
@@ -3448,9 +3639,21 @@
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr"/>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>15)</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>Spencer P</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr">
         <is>

</xml_diff>